<commit_message>
analaysis ready data completed!
</commit_message>
<xml_diff>
--- a/documents/datadictionary/EMR_data_description.xlsx
+++ b/documents/datadictionary/EMR_data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djlemas\Dropbox (UFL)\02_Projects\UFHEALTH\pe_prediction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a87caf6b30614cd/Documents/ehr-preeclampsia-model/documents/datadictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D424E758-B824-4DBB-AF27-8A26AC7A5B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{D424E758-B824-4DBB-AF27-8A26AC7A5B7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16637C94-1636-4480-94AC-D9090F15AFBC}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="1500" windowWidth="18420" windowHeight="11835" xr2:uid="{B731CDC5-07EE-6F4B-B732-086B076E6EB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B731CDC5-07EE-6F4B-B732-086B076E6EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="127">
   <si>
     <t>Variable Name</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Missing values are not allowed in the dataset. Missing values need to be imputed or removed before running the model.</t>
+  </si>
+  <si>
+    <t>Base-Model</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -779,48 +785,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D46A5E-4D51-6146-9137-9E92AA68342B}">
-  <dimension ref="A1:Y60"/>
+  <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.875" customWidth="1"/>
-    <col min="2" max="2" width="79.875" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.875" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -846,22 +853,22 @@
       <c r="M2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -887,22 +894,22 @@
       <c r="M3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
@@ -931,22 +938,22 @@
       <c r="N4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
@@ -975,22 +982,22 @@
       <c r="N5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -1016,22 +1023,22 @@
       <c r="M6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -1051,22 +1058,22 @@
       <c r="K7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F8" t="s">
         <v>5</v>
@@ -1086,22 +1093,22 @@
       <c r="K8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F9" t="s">
         <v>5</v>
@@ -1124,42 +1131,42 @@
       <c r="L9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>69</v>
       </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -1179,23 +1186,26 @@
       <c r="K11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
       <c r="F12" t="s">
         <v>5</v>
       </c>
@@ -1238,23 +1248,26 @@
       <c r="S12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
@@ -1291,23 +1304,26 @@
       <c r="Q13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" t="s">
         <v>75</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E14" t="s">
-        <v>5</v>
-      </c>
       <c r="F14" t="s">
         <v>5</v>
       </c>
@@ -1350,23 +1366,26 @@
       <c r="S14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
@@ -1406,22 +1425,22 @@
       <c r="R15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>80</v>
       </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -1450,22 +1469,22 @@
       <c r="N16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>81</v>
       </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -1491,22 +1510,22 @@
       <c r="M17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1535,42 +1554,42 @@
       <c r="N18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -1614,22 +1633,22 @@
       <c r="S20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>85</v>
       </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -1667,37 +1686,37 @@
       <c r="Q21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>87</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
       <c r="F23" t="s">
         <v>5</v>
       </c>
@@ -1758,22 +1777,22 @@
       <c r="Y23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>89</v>
       </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" t="s">
-        <v>5</v>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
@@ -1820,22 +1839,22 @@
       <c r="T24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" t="s">
-        <v>5</v>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
@@ -1879,22 +1898,22 @@
       <c r="S25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>91</v>
       </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" t="s">
-        <v>5</v>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
@@ -1932,22 +1951,22 @@
       <c r="Q26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>92</v>
       </c>
-      <c r="C27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F27" t="s">
         <v>5</v>
@@ -1979,22 +1998,22 @@
       <c r="O27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>93</v>
       </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" t="s">
-        <v>5</v>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F28" t="s">
         <v>5</v>
@@ -2041,22 +2060,22 @@
       <c r="T28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>94</v>
       </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>5</v>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
@@ -2088,22 +2107,22 @@
       <c r="O29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>95</v>
       </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" t="s">
-        <v>5</v>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F30" t="s">
         <v>5</v>
@@ -2144,22 +2163,22 @@
       <c r="R30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="C31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" t="s">
-        <v>5</v>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F31" t="s">
         <v>5</v>
@@ -2209,22 +2228,25 @@
       <c r="U31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
         <v>97</v>
       </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F32" t="s">
         <v>5</v>
@@ -2262,22 +2284,25 @@
       <c r="Q32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
       <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
         <v>98</v>
       </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" t="s">
-        <v>5</v>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F33" t="s">
         <v>5</v>
@@ -2312,22 +2337,22 @@
       <c r="P33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>99</v>
       </c>
-      <c r="C34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" t="s">
-        <v>5</v>
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F34" t="s">
         <v>5</v>
@@ -2380,22 +2405,22 @@
       <c r="V34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" t="s">
-        <v>5</v>
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F35" t="s">
         <v>5</v>
@@ -2424,22 +2449,22 @@
       <c r="N35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>101</v>
       </c>
-      <c r="C36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" t="s">
-        <v>5</v>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
@@ -2471,22 +2496,25 @@
       <c r="O36" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
         <v>102</v>
       </c>
-      <c r="C37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" t="s">
-        <v>5</v>
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
@@ -2515,22 +2543,22 @@
       <c r="N37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>103</v>
       </c>
-      <c r="C38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F38" t="s">
         <v>5</v>
@@ -2574,22 +2602,22 @@
       <c r="S38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="T38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>104</v>
       </c>
-      <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" t="s">
-        <v>5</v>
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F39" t="s">
         <v>5</v>
@@ -2636,22 +2664,22 @@
       <c r="T39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>105</v>
       </c>
-      <c r="C40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" t="s">
-        <v>5</v>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F40" t="s">
         <v>5</v>
@@ -2704,22 +2732,22 @@
       <c r="V40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>106</v>
       </c>
-      <c r="C41" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" t="s">
-        <v>5</v>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F41" t="s">
         <v>5</v>
@@ -2760,22 +2788,22 @@
       <c r="R41" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="S41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>107</v>
       </c>
-      <c r="C42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" t="s">
-        <v>5</v>
+      <c r="D42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F42" t="s">
         <v>5</v>
@@ -2831,22 +2859,22 @@
       <c r="W42" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>108</v>
       </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E43" t="s">
-        <v>5</v>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F43" t="s">
         <v>5</v>
@@ -2872,22 +2900,22 @@
       <c r="M43" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>109</v>
       </c>
-      <c r="C44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" t="s">
-        <v>5</v>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F44" t="s">
         <v>5</v>
@@ -2940,22 +2968,22 @@
       <c r="V44" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>110</v>
       </c>
-      <c r="C45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E45" t="s">
-        <v>5</v>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F45" t="s">
         <v>5</v>
@@ -2969,22 +2997,22 @@
       <c r="I45" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>111</v>
       </c>
-      <c r="C46" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" t="s">
-        <v>5</v>
+      <c r="D46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F46" t="s">
         <v>5</v>
@@ -3010,22 +3038,22 @@
       <c r="M46" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>112</v>
       </c>
-      <c r="C47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" t="s">
-        <v>5</v>
+      <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F47" t="s">
         <v>5</v>
@@ -3078,22 +3106,25 @@
       <c r="V47" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s">
         <v>113</v>
       </c>
-      <c r="C48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E48" t="s">
-        <v>5</v>
+      <c r="D48" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F48" t="s">
         <v>5</v>
@@ -3116,22 +3147,22 @@
       <c r="L48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>114</v>
       </c>
-      <c r="C49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" t="s">
-        <v>5</v>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F49" t="s">
         <v>5</v>
@@ -3178,39 +3209,39 @@
       <c r="T49" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>115</v>
       </c>
-      <c r="C50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>116</v>
       </c>
-      <c r="C51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" t="s">
-        <v>5</v>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F51" t="s">
         <v>5</v>
@@ -3236,22 +3267,22 @@
       <c r="M51" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>117</v>
       </c>
-      <c r="C52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E52" t="s">
-        <v>5</v>
+      <c r="D52" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F52" t="s">
         <v>5</v>
@@ -3295,22 +3326,22 @@
       <c r="S52" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>118</v>
       </c>
-      <c r="C53" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E53" t="s">
-        <v>5</v>
+      <c r="D53" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F53" t="s">
         <v>5</v>
@@ -3360,22 +3391,25 @@
       <c r="U53" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
       <c r="B54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" t="s">
         <v>119</v>
       </c>
-      <c r="C54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E54" t="s">
-        <v>5</v>
+      <c r="D54" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F54" t="s">
         <v>5</v>
@@ -3428,22 +3462,25 @@
       <c r="V54" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
       <c r="B55" t="s">
+        <v>126</v>
+      </c>
+      <c r="C55" t="s">
         <v>120</v>
       </c>
-      <c r="C55" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E55" t="s">
-        <v>5</v>
+      <c r="D55" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="F55" t="s">
         <v>5</v>
@@ -3454,45 +3491,52 @@
       <c r="H55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>123</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A57:E57"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>